<commit_message>
comit for the keyword driven frame work
</commit_message>
<xml_diff>
--- a/KeywordDrivenFrameworkLearning/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDrivenFrameworkLearning/src/dataEngine/DataEngine.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="5640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="3465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:I9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t xml:space="preserve">Test Case ID </t>
   </si>
@@ -116,6 +117,42 @@
   </si>
   <si>
     <t>click_Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Object </t>
+  </si>
+  <si>
+    <t>btn_MyAccount</t>
+  </si>
+  <si>
+    <t>btn_LogOut</t>
+  </si>
+  <si>
+    <t>txtbx_UserName</t>
+  </si>
+  <si>
+    <t>txtbx_Password</t>
+  </si>
+  <si>
+    <t>btn_LogIn</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login in the online Store </t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Login_02</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -444,20 +481,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" activeCellId="1" sqref="D7 D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,14 +506,17 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -485,17 +526,17 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -505,17 +546,17 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -526,16 +567,19 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -546,16 +590,19 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -566,16 +613,19 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -586,16 +636,19 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -605,17 +658,17 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -626,16 +679,19 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -645,50 +701,103 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E11" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E13" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E14" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final comit from the laptop
</commit_message>
<xml_diff>
--- a/KeywordDrivenFrameworkLearning/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDrivenFrameworkLearning/src/dataEngine/DataEngine.xlsx
@@ -4,14 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="3465" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="4980"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Settings" sheetId="3" r:id="rId2"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Action_Keywords">Settings!$D$2:$D$11</definedName>
+    <definedName name="Home_Page">Settings!$B$2:$B$11</definedName>
+    <definedName name="Login_Page">Settings!$C$2:$C$11</definedName>
+    <definedName name="Page_Name">Settings!$A$2:$A$11</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I9"/>
+  <oleSize ref="A1:E14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t xml:space="preserve">Test Case ID </t>
   </si>
@@ -92,33 +99,15 @@
     <t xml:space="preserve">Close the browser </t>
   </si>
   <si>
-    <t>OpenBrowser</t>
-  </si>
-  <si>
     <t>navigate</t>
   </si>
   <si>
-    <t>input_Username</t>
-  </si>
-  <si>
-    <t>click_Login</t>
-  </si>
-  <si>
     <t>closeBrowser</t>
   </si>
   <si>
-    <t>click_MyAccount</t>
-  </si>
-  <si>
-    <t>input_password</t>
-  </si>
-  <si>
     <t>waitFor</t>
   </si>
   <si>
-    <t>click_Logout</t>
-  </si>
-  <si>
     <t xml:space="preserve">Page Object </t>
   </si>
   <si>
@@ -152,7 +141,85 @@
     <t>Login_02</t>
   </si>
   <si>
-    <t>No</t>
+    <t>openBrowser</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Set </t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>softway_1</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
+    <t>Page Name</t>
+  </si>
+  <si>
+    <t>Login_Page Object</t>
+  </si>
+  <si>
+    <t>Home_Page Objects</t>
+  </si>
+  <si>
+    <t>Home_Page</t>
+  </si>
+  <si>
+    <t>Login_Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action Keywords </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Name </t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Mozilla</t>
+  </si>
+  <si>
+    <t>Buy_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buying product </t>
+  </si>
+  <si>
+    <t>Ts_010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open the browser </t>
+  </si>
+  <si>
+    <t>Navigate to website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on product </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enetr the product name </t>
+  </si>
+  <si>
+    <t>click on search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on buy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">input the username </t>
+  </si>
+  <si>
+    <t xml:space="preserve">input password </t>
   </si>
 </sst>
 </file>
@@ -481,21 +548,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" activeCellId="1" sqref="D7 D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="64" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="64" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,17 +574,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -526,17 +602,22 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -546,17 +627,16 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -567,19 +647,21 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -590,19 +672,24 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -613,19 +700,24 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -636,19 +728,21 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -658,17 +752,16 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -679,19 +772,21 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -701,49 +796,122 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27">
+      <formula1>Page_Name</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
+      <formula1>INDIRECT(D2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11">
+      <formula1>Action_Keywords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E28">
+      <formula1>INDIRECT(D2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -751,53 +919,155 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>